<commit_message>
CEM and First Regressions
Matching and regressions based on environmental factors
</commit_message>
<xml_diff>
--- a/Data Tracker.xlsx
+++ b/Data Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\OneDrive\Documents\Wageningen\University\Thesis\WURthesisGithub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0245BA-1FB1-401B-BB84-236A4712FBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31E6B20-9054-4AF9-8DB4-D9A7A97D162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{D36AC524-343E-4F85-A404-2DDC80872131}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="2" xr2:uid="{D36AC524-343E-4F85-A404-2DDC80872131}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -707,7 +707,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,18 +730,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1174,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793D9757-2FB6-40C8-AD98-3C3854247702}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1486,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3501D6-AAD0-457F-A2AA-309A99FC0788}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1851,7 +1839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4786E872-9DE7-4C79-97AA-C7147A82E0F6}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>

</xml_diff>